<commit_message>
Pioneer 6 Deployment Cal Sheets
Updated Cal Info Sheets for moorings deployed on Pioneer 6.
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP02PMCI_00005.xlsx
+++ b/deployment/Omaha_Cal_Info_CP02PMCI_00005.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="3820" windowWidth="24500" windowHeight="13840" tabRatio="377"/>
+    <workbookView xWindow="3080" yWindow="1500" windowWidth="27100" windowHeight="16560" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>Ref Des</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>SWE 0008 Rev G</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -288,6 +291,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="55"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -384,7 +399,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -436,8 +451,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -458,9 +484,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,12 +526,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="62">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -534,6 +565,11 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -559,7 +595,13 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Asset_Cal_Info" xfId="55"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -932,7 +974,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -950,76 +992,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="15" t="s">
+      <c r="H1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="16">
-        <v>5</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
+      <c r="C2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="15">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16">
+        <v>42511</v>
+      </c>
+      <c r="F2" s="17">
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="G2" s="16">
+        <v>42520</v>
+      </c>
+      <c r="H2" s="12">
+        <v>40.226550000000003</v>
+      </c>
+      <c r="I2" s="12">
+        <v>-70.888966666666661</v>
+      </c>
+      <c r="J2" s="12">
+        <v>128</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="11" t="e">
-        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N2" s="3" t="e">
-        <f>((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="L2" s="18"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:14">
       <c r="E4" s="2"/>
@@ -1041,7 +1090,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1084,7 +1133,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="5"/>
@@ -1095,20 +1144,22 @@
         <v>5</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>19151</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="27"/>
+      <c r="H2" s="27">
+        <v>105000</v>
+      </c>
       <c r="I2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="5"/>
@@ -1119,18 +1170,20 @@
         <v>5</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <v>19151</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="28">
+        <v>40.226550000000003</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="5"/>
@@ -1141,13 +1194,15 @@
         <v>5</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>19151</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="27"/>
+      <c r="H4" s="28">
+        <v>-70.888966666666661</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
@@ -1157,7 +1212,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="21"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -1175,7 +1230,9 @@
         <v>5</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="29" t="s">
+        <v>57</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1183,7 +1240,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="E7" s="2"/>
-      <c r="F7" s="22"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
@@ -1197,13 +1254,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>54</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="25">
         <v>-848.41</v>
       </c>
       <c r="I8" s="4"/>
@@ -1221,13 +1278,15 @@
         <v>5</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="20" t="s">
         <v>54</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="27"/>
+      <c r="H9" s="28">
+        <v>40.226550000000003</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
@@ -1243,13 +1302,15 @@
         <v>5</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="20" t="s">
         <v>54</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="28">
+        <v>-70.888966666666661</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
@@ -1265,13 +1326,13 @@
         <v>5</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>54</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="24">
         <v>3.1689000000000001E-4</v>
       </c>
       <c r="I11" s="4"/>
@@ -1289,13 +1350,13 @@
         <v>5</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="20" t="s">
         <v>54</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="24">
         <v>-3.0266E-3</v>
       </c>
       <c r="I12" s="4"/>
@@ -1313,13 +1374,13 @@
         <v>5</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="20" t="s">
         <v>54</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="24">
         <v>1.7720999999999999E-4</v>
       </c>
       <c r="I13" s="4"/>
@@ -1337,13 +1398,13 @@
         <v>5</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="20" t="s">
         <v>54</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="24">
         <v>-3.2445999999999998E-6</v>
       </c>
       <c r="I14" s="4"/>
@@ -1361,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="20" t="s">
         <v>54</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="24">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I15" s="4"/>
@@ -1379,7 +1440,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="22"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="4"/>
       <c r="H16" s="6"/>
       <c r="I16" s="4"/>
@@ -1397,13 +1458,15 @@
         <v>5</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <v>113</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="27"/>
+      <c r="H17" s="28">
+        <v>40.226550000000003</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
@@ -1419,13 +1482,15 @@
         <v>5</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="21">
+      <c r="F18" s="20">
         <v>113</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="27"/>
+      <c r="H18" s="28">
+        <v>-70.888966666666661</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
@@ -1435,7 +1500,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="22"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -1453,13 +1518,15 @@
         <v>5</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="21">
+      <c r="F20" s="20">
         <v>100013</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="27"/>
+      <c r="H20" s="28">
+        <v>40.226550000000003</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
@@ -1475,13 +1542,15 @@
         <v>5</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="21">
+      <c r="F21" s="20">
         <v>100013</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="27"/>
+      <c r="H21" s="28">
+        <v>-70.888966666666661</v>
+      </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
@@ -1491,7 +1560,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="22"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1509,7 +1578,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="21">
+      <c r="F23" s="20">
         <v>1031</v>
       </c>
       <c r="G23" s="4" t="s">
@@ -1535,13 +1604,13 @@
         <v>5</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="21">
+      <c r="F24" s="20">
         <v>1031</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="22">
         <v>47</v>
       </c>
       <c r="I24" s="5"/>
@@ -1559,13 +1628,13 @@
         <v>5</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="21">
+      <c r="F25" s="20">
         <v>1031</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="22">
         <v>46</v>
       </c>
       <c r="I25" s="5"/>
@@ -1583,13 +1652,13 @@
         <v>5</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="21">
+      <c r="F26" s="20">
         <v>1031</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="22">
         <v>49</v>
       </c>
       <c r="I26" s="4"/>
@@ -1607,7 +1676,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="21">
+      <c r="F27" s="20">
         <v>1031</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -1633,7 +1702,7 @@
         <v>5</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="21">
+      <c r="F28" s="20">
         <v>1031</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -1659,16 +1728,16 @@
         <v>5</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="21">
+      <c r="F29" s="20">
         <v>1031</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="23">
+      <c r="H29" s="22">
         <v>7.2300000000000003E-2</v>
       </c>
-      <c r="I29" s="20"/>
+      <c r="I29" s="19"/>
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10">
@@ -1683,13 +1752,13 @@
         <v>5</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="21">
+      <c r="F30" s="20">
         <v>1031</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H30" s="23">
+      <c r="H30" s="22">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="I30" s="4"/>
@@ -1707,13 +1776,13 @@
         <v>5</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="21">
+      <c r="F31" s="20">
         <v>1031</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="23">
+      <c r="H31" s="22">
         <v>3.1540000000000002E-6</v>
       </c>
       <c r="I31" s="4"/>
@@ -1731,7 +1800,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="21">
+      <c r="F32" s="20">
         <v>1031</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -1751,7 +1820,7 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="22"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -1769,13 +1838,13 @@
         <v>5</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="21">
+      <c r="F34" s="20">
         <v>20447</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="23">
+      <c r="H34" s="22">
         <v>0.9</v>
       </c>
       <c r="I34" s="4"/>
@@ -1793,13 +1862,13 @@
         <v>5</v>
       </c>
       <c r="E35" s="2"/>
-      <c r="F35" s="21">
+      <c r="F35" s="20">
         <v>20447</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H35" s="24">
+      <c r="H35" s="23">
         <v>1.13E-17</v>
       </c>
       <c r="I35" s="4"/>
@@ -1810,8 +1879,8 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="22"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -1829,7 +1898,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="21" t="s">
         <v>55</v>
       </c>
       <c r="G37" s="4"/>
@@ -1839,7 +1908,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="E38" s="2"/>
-      <c r="F38" s="22"/>
+      <c r="F38" s="21"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="4" t="s">
@@ -1853,7 +1922,7 @@
         <v>5</v>
       </c>
       <c r="E39" s="5"/>
-      <c r="F39" s="28" t="s">
+      <c r="F39" s="26" t="s">
         <v>56</v>
       </c>
       <c r="G39" s="4"/>
@@ -1862,7 +1931,7 @@
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="F40" s="28"/>
+      <c r="F40" s="26"/>
     </row>
     <row r="41" spans="1:10">
       <c r="F41" s="9"/>

</xml_diff>

<commit_message>
CP02PMCI D5 Calibration and ingest
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP02PMCI_00005.xlsx
+++ b/deployment/Omaha_Cal_Info_CP02PMCI_00005.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="1500" windowWidth="27100" windowHeight="16560" tabRatio="377"/>
+    <workbookView xWindow="3075" yWindow="1500" windowWidth="27105" windowHeight="16560" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$76</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$405</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="68">
   <si>
     <t>Ref Des</t>
   </si>
@@ -213,7 +218,37 @@
     <t>SWE 0008 Rev G</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>OL000237</t>
+  </si>
+  <si>
+    <t>A00234</t>
+  </si>
+  <si>
+    <t>CP02PMCI-00005-MOPAK</t>
+  </si>
+  <si>
+    <t>OL000238</t>
+  </si>
+  <si>
+    <t>N00037</t>
+  </si>
+  <si>
+    <t>N00036</t>
+  </si>
+  <si>
+    <t>N00041</t>
+  </si>
+  <si>
+    <t>N00038</t>
+  </si>
+  <si>
+    <t>N00040</t>
+  </si>
+  <si>
+    <t>A00286</t>
+  </si>
+  <si>
+    <t>OL000239</t>
   </si>
 </sst>
 </file>
@@ -223,7 +258,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -284,6 +319,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -299,14 +335,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,12 +352,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,7 +487,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -535,8 +559,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -973,25 +1000,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="9" width="19.83203125" customWidth="1"/>
-    <col min="10" max="10" width="9.83203125" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28">
+    <row r="1" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>49</v>
       </c>
@@ -1029,8 +1056,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="15"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
       <c r="B2" s="15" t="s">
         <v>35</v>
       </c>
@@ -1065,12 +1094,12 @@
       <c r="M2" s="10"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
@@ -1087,26 +1116,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1132,18 +1161,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
       <c r="C2" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="5">
         <v>5</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
       <c r="F2" s="20">
         <v>19151</v>
       </c>
@@ -1156,20 +1189,24 @@
       <c r="I2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="N2" s="29"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="5">
         <v>5</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
       <c r="F3" s="20">
         <v>19151</v>
       </c>
@@ -1180,20 +1217,24 @@
         <v>40.226550000000003</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="N3" s="29"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="5">
         <v>5</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
       <c r="F4" s="20">
         <v>19151</v>
       </c>
@@ -1204,9 +1245,9 @@
         <v>-70.888966666666661</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="N4" s="29"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -1216,44 +1257,53 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="N5" s="29"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
       <c r="C6" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="29" t="s">
-        <v>57</v>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="N6" s="29"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="N7" s="29"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
       <c r="C8" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
       <c r="F8" s="20" t="s">
         <v>54</v>
       </c>
@@ -1264,20 +1314,24 @@
         <v>-848.41</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="N8" s="29"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="5">
         <v>5</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
       <c r="F9" s="20" t="s">
         <v>54</v>
       </c>
@@ -1288,20 +1342,24 @@
         <v>40.226550000000003</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="N9" s="29"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
       <c r="C10" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="5">
         <v>5</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
       <c r="F10" s="20" t="s">
         <v>54</v>
       </c>
@@ -1312,20 +1370,24 @@
         <v>-70.888966666666661</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="N10" s="29"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
       <c r="C11" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="5">
         <v>5</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
       <c r="F11" s="20" t="s">
         <v>54</v>
       </c>
@@ -1336,20 +1398,24 @@
         <v>3.1689000000000001E-4</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="N11" s="29"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
       <c r="C12" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="20" t="s">
         <v>54</v>
       </c>
@@ -1360,20 +1426,23 @@
         <v>-3.0266E-3</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
       <c r="C13" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="5">
         <v>5</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="20" t="s">
         <v>54</v>
       </c>
@@ -1384,20 +1453,23 @@
         <v>1.7720999999999999E-4</v>
       </c>
       <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="5">
         <v>5</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
       <c r="F14" s="20" t="s">
         <v>54</v>
       </c>
@@ -1408,20 +1480,23 @@
         <v>-3.2445999999999998E-6</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
       <c r="C15" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="5">
         <v>5</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
       <c r="F15" s="20" t="s">
         <v>54</v>
       </c>
@@ -1432,9 +1507,8 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -1444,20 +1518,23 @@
       <c r="G16" s="4"/>
       <c r="H16" s="6"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
       <c r="C17" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="5">
         <v>5</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
       <c r="F17" s="20">
         <v>113</v>
       </c>
@@ -1468,20 +1545,23 @@
         <v>40.226550000000003</v>
       </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
       <c r="C18" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="5">
         <v>5</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
       <c r="F18" s="20">
         <v>113</v>
       </c>
@@ -1492,9 +1572,8 @@
         <v>-70.888966666666661</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
@@ -1504,20 +1583,23 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
       <c r="C20" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D20" s="5">
         <v>5</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
       <c r="F20" s="20">
         <v>100013</v>
       </c>
@@ -1528,20 +1610,23 @@
         <v>40.226550000000003</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
       <c r="C21" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="5">
         <v>5</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
       <c r="F21" s="20">
         <v>100013</v>
       </c>
@@ -1552,9 +1637,8 @@
         <v>-70.888966666666661</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -1564,20 +1648,23 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
       <c r="C23" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="5">
         <v>5</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
       <c r="F23" s="20">
         <v>1031</v>
       </c>
@@ -1590,20 +1677,23 @@
       <c r="I23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
       <c r="C24" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="5">
         <v>5</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" t="s">
+        <v>64</v>
+      </c>
       <c r="F24" s="20">
         <v>1031</v>
       </c>
@@ -1614,20 +1704,23 @@
         <v>47</v>
       </c>
       <c r="I24" s="5"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
       <c r="C25" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="5">
         <v>5</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
       <c r="F25" s="20">
         <v>1031</v>
       </c>
@@ -1638,20 +1731,23 @@
         <v>46</v>
       </c>
       <c r="I25" s="5"/>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
       <c r="C26" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D26" s="5">
         <v>5</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
       <c r="F26" s="20">
         <v>1031</v>
       </c>
@@ -1662,20 +1758,23 @@
         <v>49</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
       <c r="C27" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="5">
         <v>5</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
       <c r="F27" s="20">
         <v>1031</v>
       </c>
@@ -1688,20 +1787,23 @@
       <c r="I27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
       <c r="C28" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="5">
         <v>5</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
       <c r="F28" s="20">
         <v>1031</v>
       </c>
@@ -1714,20 +1816,23 @@
       <c r="I28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D29" s="5">
         <v>5</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" t="s">
+        <v>64</v>
+      </c>
       <c r="F29" s="20">
         <v>1031</v>
       </c>
@@ -1738,20 +1843,23 @@
         <v>7.2300000000000003E-2</v>
       </c>
       <c r="I29" s="19"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D30" s="5">
         <v>5</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" t="s">
+        <v>64</v>
+      </c>
       <c r="F30" s="20">
         <v>1031</v>
       </c>
@@ -1762,20 +1870,23 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
       <c r="C31" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D31" s="5">
         <v>5</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
       <c r="F31" s="20">
         <v>1031</v>
       </c>
@@ -1786,20 +1897,23 @@
         <v>3.1540000000000002E-6</v>
       </c>
       <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
       <c r="C32" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="5">
         <v>5</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" t="s">
+        <v>64</v>
+      </c>
       <c r="F32" s="20">
         <v>1031</v>
       </c>
@@ -1812,9 +1926,8 @@
       <c r="I32" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
@@ -1824,22 +1937,25 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="5"/>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
       <c r="C34" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D34" s="5">
         <v>5</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
       <c r="F34" s="20">
-        <v>20447</v>
+        <v>20477</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>31</v>
@@ -1848,22 +1964,25 @@
         <v>0.9</v>
       </c>
       <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
       <c r="C35" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D35" s="5">
         <v>5</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" t="s">
+        <v>65</v>
+      </c>
       <c r="F35" s="20">
-        <v>20447</v>
+        <v>20477</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>32</v>
@@ -1872,9 +1991,8 @@
         <v>1.13E-17</v>
       </c>
       <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1884,62 +2002,67 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="5"/>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
       <c r="C37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D37" s="5">
         <v>5</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="30" t="s">
+        <v>66</v>
+      </c>
       <c r="F37" s="21" t="s">
         <v>55</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E38" s="2"/>
       <c r="F38" s="21"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
       <c r="C39" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D39" s="5">
         <v>5</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" t="s">
+        <v>67</v>
+      </c>
       <c r="F39" s="26" t="s">
         <v>56</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F40" s="26"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F43" s="9"/>
     </row>
   </sheetData>

</xml_diff>